<commit_message>
Update Non-Archetype Demands, 2018 Retrofits, WAM 2050 target, Coal&Peat Phase-down
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_RSD-Retrofit.xlsx
+++ b/SubRES_TMPL/SubRES_RSD-Retrofit.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB89D5BA-A3C0-45D7-B556-2D9E096134DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B38A62-35F6-4C4B-B97D-8106B39745BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12780" yWindow="-16380" windowWidth="29040" windowHeight="15840" xr2:uid="{61E3DBC4-3D48-40CE-BDD5-C17192DCDA09}"/>
+    <workbookView xWindow="16020" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{61E3DBC4-3D48-40CE-BDD5-C17192DCDA09}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="59" r:id="rId1"/>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -3888,7 +3888,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:Z99"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B26" sqref="B26:D26"/>
     </sheetView>
   </sheetViews>
@@ -8279,8 +8279,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AP60"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="W39" sqref="W39"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9560,16 +9560,16 @@
         <v>185</v>
       </c>
       <c r="F18" s="112">
-        <f>SUM(D5:D8)</f>
-        <v>92323.794764485472</v>
+        <f>SUM(D5:D7)</f>
+        <v>42554.945078555997</v>
       </c>
       <c r="G18" s="112">
-        <f>SUM(E5:E8)</f>
-        <v>103369.76677783766</v>
+        <f t="shared" ref="G18:H18" si="8">SUM(E5:E7)</f>
+        <v>49903.556733855992</v>
       </c>
       <c r="H18" s="112">
-        <f>SUM(F5:F8)</f>
-        <v>50844.518002144141</v>
+        <f t="shared" si="8"/>
+        <v>30920.037627088317</v>
       </c>
       <c r="L18" s="104" t="s">
         <v>169</v>
@@ -9581,15 +9581,15 @@
         <v>111</v>
       </c>
       <c r="P18" s="173">
-        <f t="shared" ref="P18:P25" si="8">1-W4/$W$12</f>
+        <f t="shared" ref="P18:P25" si="9">1-W4/$W$12</f>
         <v>0.82657317923529827</v>
       </c>
       <c r="Q18" s="174">
-        <f t="shared" ref="Q18:Q24" si="9">1-W4/$W$11</f>
+        <f t="shared" ref="Q18:Q24" si="10">1-W4/$W$11</f>
         <v>0.73202753715113</v>
       </c>
       <c r="R18" s="174">
-        <f t="shared" ref="R18:R23" si="10">1-W4/$W$10</f>
+        <f t="shared" ref="R18:R23" si="11">1-W4/$W$10</f>
         <v>0.67174081354445081</v>
       </c>
       <c r="S18" s="174">
@@ -9658,30 +9658,30 @@
         <v>186</v>
       </c>
       <c r="F19" s="112">
-        <f>D9</f>
-        <v>282151.52747564798</v>
+        <f>SUM(D8:D10)</f>
+        <v>519547.39953818789</v>
       </c>
       <c r="G19" s="112">
-        <f t="shared" ref="G19:H19" si="11">E9</f>
-        <v>251318.93361374349</v>
+        <f t="shared" ref="G19:H19" si="12">SUM(E8:E10)</f>
+        <v>471452.93507051643</v>
       </c>
       <c r="H19" s="112">
-        <f t="shared" si="11"/>
-        <v>58904.8034364337</v>
+        <f t="shared" si="12"/>
+        <v>122568.62546059568</v>
       </c>
       <c r="O19" s="84" t="s">
         <v>114</v>
       </c>
       <c r="P19" s="173">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.79158454239957576</v>
       </c>
       <c r="Q19" s="174">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.67796443927935268</v>
       </c>
       <c r="R19" s="174">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.60551494714016629</v>
       </c>
       <c r="S19" s="174">
@@ -9747,30 +9747,30 @@
         <v>187</v>
       </c>
       <c r="F20" s="112">
-        <f>SUM(D10:D13)</f>
-        <v>391876.39875986642</v>
+        <f>SUM(D11:D13)</f>
+        <v>204249.37638325599</v>
       </c>
       <c r="G20" s="112">
-        <f t="shared" ref="G20:H20" si="12">SUM(E10:E13)</f>
-        <v>369741.02860841871</v>
+        <f t="shared" ref="G20:H20" si="13">SUM(E11:E13)</f>
+        <v>203073.23719562744</v>
       </c>
       <c r="H20" s="112">
-        <f t="shared" si="12"/>
-        <v>97049.563561422125</v>
+        <f t="shared" si="13"/>
+        <v>53310.221912315974</v>
       </c>
       <c r="O20" s="89" t="s">
         <v>115</v>
       </c>
       <c r="P20" s="174">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.73294667697694738</v>
       </c>
       <c r="Q20" s="174">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.58735946166276198</v>
       </c>
       <c r="R20" s="174">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.49452624358065522</v>
       </c>
       <c r="S20" s="175">
@@ -9801,15 +9801,15 @@
         <v>116</v>
       </c>
       <c r="P21" s="174">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.67711162025267657</v>
       </c>
       <c r="Q21" s="174">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.50108527640274758</v>
       </c>
       <c r="R21" s="174">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.38884264622707332</v>
       </c>
       <c r="S21" s="175">
@@ -9841,15 +9841,15 @@
         <v>118</v>
       </c>
       <c r="P22" s="174">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.72141928210057427</v>
       </c>
       <c r="Q22" s="174">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.56954777381867572</v>
       </c>
       <c r="R22" s="174">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.47270739660309302</v>
       </c>
       <c r="S22" s="175">
@@ -9867,29 +9867,29 @@
       </c>
       <c r="F23" s="131">
         <f>F18/$D$14</f>
-        <v>0.12047183066805627</v>
+        <v>5.5529261450638807E-2</v>
       </c>
       <c r="G23" s="131">
         <f>G18/$E$14</f>
-        <v>0.14269122682268837</v>
+        <v>6.8886676976582226E-2</v>
       </c>
       <c r="H23" s="131">
         <f>H18/$F$14</f>
-        <v>0.24586456547937455</v>
+        <v>0.14951742910552115</v>
       </c>
       <c r="O23" s="84" t="s">
         <v>122</v>
       </c>
       <c r="P23" s="174">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.60126424040662463</v>
       </c>
       <c r="Q23" s="174">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.38388881804434616</v>
       </c>
       <c r="R23" s="175">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.24528008137541124</v>
       </c>
       <c r="S23" s="173"/>
@@ -9903,26 +9903,26 @@
         <v>186</v>
       </c>
       <c r="F24" s="131">
-        <f t="shared" ref="F24:F25" si="13">F19/$D$14</f>
-        <v>0.36817497729041837</v>
+        <f t="shared" ref="F24:F25" si="14">F19/$D$14</f>
+        <v>0.67794902171060434</v>
       </c>
       <c r="G24" s="131">
-        <f t="shared" ref="G24:G25" si="14">G19/$E$14</f>
-        <v>0.34691968530979972</v>
+        <f t="shared" ref="G24:G25" si="15">G19/$E$14</f>
+        <v>0.65079181071338454</v>
       </c>
       <c r="H24" s="131">
-        <f t="shared" ref="H24:H25" si="15">H19/$F$14</f>
-        <v>0.28484101080348528</v>
+        <f t="shared" ref="H24:H25" si="16">H19/$F$14</f>
+        <v>0.59269480810109632</v>
       </c>
       <c r="O24" s="89" t="s">
         <v>125</v>
       </c>
       <c r="P24" s="174">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.47167717486503269</v>
       </c>
       <c r="Q24" s="175">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.18365586126511313</v>
       </c>
       <c r="R24" s="173"/>
@@ -9937,22 +9937,22 @@
         <v>187</v>
       </c>
       <c r="F25" s="131">
-        <f t="shared" si="13"/>
-        <v>0.51135319204152541</v>
+        <f t="shared" si="14"/>
+        <v>0.26652171683875692</v>
       </c>
       <c r="G25" s="131">
-        <f t="shared" si="14"/>
-        <v>0.5103890878675118</v>
+        <f t="shared" si="15"/>
+        <v>0.28032151231003311</v>
       </c>
       <c r="H25" s="131">
-        <f t="shared" si="15"/>
-        <v>0.46929442371714014</v>
+        <f t="shared" si="16"/>
+        <v>0.25778776279338245</v>
       </c>
       <c r="O25" s="84" t="s">
         <v>127</v>
       </c>
       <c r="P25" s="175">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.3528184988824381</v>
       </c>
       <c r="Q25" s="175"/>
@@ -10094,7 +10094,7 @@
         <v>6086</v>
       </c>
       <c r="G31" s="113">
-        <f t="shared" ref="G31:G56" si="16">SUM(E31:F31)</f>
+        <f t="shared" ref="G31:G56" si="17">SUM(E31:F31)</f>
         <v>21064</v>
       </c>
       <c r="H31" s="113"/>
@@ -10103,7 +10103,7 @@
       <c r="K31" s="113"/>
       <c r="L31" s="113"/>
       <c r="M31" s="113">
-        <f t="shared" ref="M31:M44" si="17">AVERAGE(G31:I31)</f>
+        <f t="shared" ref="M31:M44" si="18">AVERAGE(G31:I31)</f>
         <v>21064</v>
       </c>
       <c r="N31" s="113">
@@ -10133,7 +10133,7 @@
         <v>6086</v>
       </c>
       <c r="G32" s="114">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>30424</v>
       </c>
       <c r="H32" s="114"/>
@@ -10142,15 +10142,15 @@
       <c r="K32" s="114"/>
       <c r="L32" s="114"/>
       <c r="M32" s="114">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>30424</v>
       </c>
       <c r="N32" s="114">
-        <f t="shared" ref="N32:N57" si="18">AVERAGE(G32*1.1,J32:K32)</f>
+        <f t="shared" ref="N32:N57" si="19">AVERAGE(G32*1.1,J32:K32)</f>
         <v>33466.400000000001</v>
       </c>
       <c r="O32" s="114">
-        <f t="shared" ref="O32:O57" si="19">AVERAGE(G32*0.9,L32)</f>
+        <f t="shared" ref="O32:O57" si="20">AVERAGE(G32*0.9,L32)</f>
         <v>27381.600000000002</v>
       </c>
       <c r="P32" s="119"/>
@@ -10172,7 +10172,7 @@
         <v>6086</v>
       </c>
       <c r="G33" s="114">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>30424</v>
       </c>
       <c r="H33" s="114"/>
@@ -10181,15 +10181,15 @@
       <c r="K33" s="114"/>
       <c r="L33" s="114"/>
       <c r="M33" s="114">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>30424</v>
       </c>
       <c r="N33" s="114">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>33466.400000000001</v>
       </c>
       <c r="O33" s="114">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>27381.600000000002</v>
       </c>
       <c r="P33" s="119"/>
@@ -10214,7 +10214,7 @@
         <v>6086</v>
       </c>
       <c r="G34" s="114">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>32297</v>
       </c>
       <c r="H34" s="114"/>
@@ -10223,15 +10223,15 @@
       <c r="K34" s="114"/>
       <c r="L34" s="114"/>
       <c r="M34" s="114">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>32297</v>
       </c>
       <c r="N34" s="114">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>35526.700000000004</v>
       </c>
       <c r="O34" s="114">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>29067.3</v>
       </c>
       <c r="P34" s="119"/>
@@ -10253,7 +10253,7 @@
         <v>6086</v>
       </c>
       <c r="G35" s="114">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>34169</v>
       </c>
       <c r="H35" s="114"/>
@@ -10262,15 +10262,15 @@
       <c r="K35" s="114"/>
       <c r="L35" s="114"/>
       <c r="M35" s="114">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>34169</v>
       </c>
       <c r="N35" s="114">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>37585.9</v>
       </c>
       <c r="O35" s="114">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>30752.100000000002</v>
       </c>
       <c r="P35" s="119"/>
@@ -10292,7 +10292,7 @@
         <v>6086</v>
       </c>
       <c r="G36" s="114">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>36041</v>
       </c>
       <c r="H36" s="114"/>
@@ -10301,15 +10301,15 @@
       <c r="K36" s="114"/>
       <c r="L36" s="114"/>
       <c r="M36" s="114">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>36041</v>
       </c>
       <c r="N36" s="114">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>39645.100000000006</v>
       </c>
       <c r="O36" s="114">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>32436.9</v>
       </c>
       <c r="P36" s="119"/>
@@ -10331,7 +10331,7 @@
         <v>6086</v>
       </c>
       <c r="G37" s="115">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>21064</v>
       </c>
       <c r="H37" s="115"/>
@@ -10340,11 +10340,11 @@
       <c r="K37" s="115"/>
       <c r="L37" s="115"/>
       <c r="M37" s="115">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>21064</v>
       </c>
       <c r="N37" s="115">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>23170.400000000001</v>
       </c>
       <c r="O37" s="115">
@@ -10400,7 +10400,7 @@
         <v>6086</v>
       </c>
       <c r="G38" s="113">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>30424</v>
       </c>
       <c r="H38" s="113"/>
@@ -10409,15 +10409,15 @@
       <c r="K38" s="113"/>
       <c r="L38" s="113"/>
       <c r="M38" s="113">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>30424</v>
       </c>
       <c r="N38" s="113">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>33466.400000000001</v>
       </c>
       <c r="O38" s="113">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>27381.600000000002</v>
       </c>
       <c r="P38" s="121">
@@ -10437,11 +10437,11 @@
         <v>11432.162401919726</v>
       </c>
       <c r="T38" s="113">
-        <f t="shared" ref="T38:U38" si="20">SUM(E9)/SUM(E6:E13)*N38</f>
+        <f t="shared" ref="T38:U38" si="21">SUM(E9)/SUM(E6:E13)*N38</f>
         <v>11946.208000785055</v>
       </c>
       <c r="U38" s="113">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>8171.5871871879508</v>
       </c>
       <c r="V38" s="121">
@@ -10469,7 +10469,7 @@
         <v>5326</v>
       </c>
       <c r="G39" s="115">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>12815</v>
       </c>
       <c r="H39" s="115">
@@ -10484,7 +10484,7 @@
         <v>9007.5</v>
       </c>
       <c r="N39" s="115">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>14096.500000000002</v>
       </c>
       <c r="O39" s="115">
@@ -10520,11 +10520,11 @@
         <v>2.6971994278870277E-2</v>
       </c>
       <c r="W39" s="120">
-        <f t="shared" ref="W39:X39" si="21">E9/SUM(E6:E13)*Q39</f>
+        <f t="shared" ref="W39:X39" si="22">E9/SUM(E6:E13)*Q39</f>
         <v>2.9442086985843354E-2</v>
       </c>
       <c r="X39" s="120">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1.6202273564329378E-2</v>
       </c>
     </row>
@@ -10540,7 +10540,7 @@
         <v>6086</v>
       </c>
       <c r="G40" s="114">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>30424</v>
       </c>
       <c r="H40" s="114"/>
@@ -10549,15 +10549,15 @@
       <c r="K40" s="114"/>
       <c r="L40" s="114"/>
       <c r="M40" s="114">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>30424</v>
       </c>
       <c r="N40" s="114">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>33466.400000000001</v>
       </c>
       <c r="O40" s="114">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>27381.600000000002</v>
       </c>
       <c r="P40" s="122">
@@ -10609,7 +10609,7 @@
         <v>5326</v>
       </c>
       <c r="G41" s="113">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>12815</v>
       </c>
       <c r="H41" s="113"/>
@@ -10618,15 +10618,15 @@
       <c r="K41" s="113"/>
       <c r="L41" s="113"/>
       <c r="M41" s="113">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>12815</v>
       </c>
       <c r="N41" s="113">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>14096.500000000002</v>
       </c>
       <c r="O41" s="113">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>11533.5</v>
       </c>
       <c r="P41" s="121">
@@ -10646,11 +10646,11 @@
         <v>3202.1646884279426</v>
       </c>
       <c r="T41" s="113">
-        <f t="shared" ref="T41:U41" si="22">SUM(E10)/SUM(E6:E13)*N41</f>
+        <f t="shared" ref="T41:U41" si="23">SUM(E10)/SUM(E6:E13)*N41</f>
         <v>3337.0202528302325</v>
       </c>
       <c r="U41" s="113">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>2555.819902348102</v>
       </c>
       <c r="V41" s="121">
@@ -10658,11 +10658,11 @@
         <v>9.8677408120900534E-2</v>
       </c>
       <c r="W41" s="121">
-        <f t="shared" ref="W41:X41" si="23">SUM(E10)/SUM(E6:E13)*Q41</f>
+        <f t="shared" ref="W41:X41" si="24">SUM(E10)/SUM(E6:E13)*Q41</f>
         <v>9.5303763892583535E-2</v>
       </c>
       <c r="X41" s="121">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>8.1230839111318301E-2</v>
       </c>
     </row>
@@ -10678,7 +10678,7 @@
         <v>4565</v>
       </c>
       <c r="G42" s="115">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>8309</v>
       </c>
       <c r="H42" s="115">
@@ -10693,15 +10693,15 @@
       <c r="K42" s="115"/>
       <c r="L42" s="115"/>
       <c r="M42" s="115">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>7536.333333333333</v>
       </c>
       <c r="N42" s="115">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>19569.95</v>
       </c>
       <c r="O42" s="115">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>7478.1</v>
       </c>
       <c r="P42" s="120">
@@ -10733,11 +10733,11 @@
         <v>8.6985148229525189E-2</v>
       </c>
       <c r="W42" s="120">
-        <f t="shared" ref="W42:X42" si="24">E10/SUM(E6:E13)*Q42</f>
+        <f t="shared" ref="W42:X42" si="25">E10/SUM(E6:E13)*Q42</f>
         <v>8.2590641405322962E-2</v>
       </c>
       <c r="X42" s="120">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>7.3172573402951982E-2</v>
       </c>
     </row>
@@ -10753,7 +10753,7 @@
         <v>6086</v>
       </c>
       <c r="G43" s="114">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>32297</v>
       </c>
       <c r="H43" s="114"/>
@@ -10762,15 +10762,15 @@
       <c r="K43" s="114"/>
       <c r="L43" s="114"/>
       <c r="M43" s="114">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>32297</v>
       </c>
       <c r="N43" s="114">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>35526.700000000004</v>
       </c>
       <c r="O43" s="114">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>29067.3</v>
       </c>
       <c r="P43" s="122">
@@ -10790,11 +10790,11 @@
         <v>4362.2517866563512</v>
       </c>
       <c r="T43" s="113">
-        <f t="shared" ref="T43" si="25">SUM(E$11)/SUM(E$6:E$13)*N43</f>
+        <f t="shared" ref="T43" si="26">SUM(E$11)/SUM(E$6:E$13)*N43</f>
         <v>4107.3103757879071</v>
       </c>
       <c r="U43" s="113">
-        <f t="shared" ref="U43" si="26">SUM(F$11)/SUM(F$6:F$13)*O43</f>
+        <f t="shared" ref="U43" si="27">SUM(F$11)/SUM(F$6:F$13)*O43</f>
         <v>3794.7241279737277</v>
       </c>
       <c r="V43" s="121">
@@ -10802,11 +10802,11 @@
         <v>9.7314197405272987E-2</v>
       </c>
       <c r="W43" s="121">
-        <f t="shared" ref="W43" si="27">SUM(E$11)/SUM(E$6:E$13)*Q43</f>
+        <f t="shared" ref="W43" si="28">SUM(E$11)/SUM(E$6:E$13)*Q43</f>
         <v>8.3896324072304435E-2</v>
       </c>
       <c r="X43" s="121">
-        <f t="shared" ref="X43" si="28">SUM(F$11)/SUM(F$6:F$13)*R43</f>
+        <f t="shared" ref="X43" si="29">SUM(F$11)/SUM(F$6:F$13)*R43</f>
         <v>9.234697345696842E-2</v>
       </c>
     </row>
@@ -10822,7 +10822,7 @@
         <v>5326</v>
       </c>
       <c r="G44" s="113">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>20304</v>
       </c>
       <c r="H44" s="113"/>
@@ -10831,15 +10831,15 @@
       <c r="K44" s="113"/>
       <c r="L44" s="113"/>
       <c r="M44" s="113">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>20304</v>
       </c>
       <c r="N44" s="113">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>22334.400000000001</v>
       </c>
       <c r="O44" s="113">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>18273.600000000002</v>
       </c>
       <c r="P44" s="121">
@@ -10859,11 +10859,11 @@
         <v>2742.3958967170497</v>
       </c>
       <c r="T44" s="113">
-        <f t="shared" ref="T44:U44" si="29">SUM(E$11)/SUM(E$6:E$13)*N44</f>
+        <f t="shared" ref="T44:U44" si="30">SUM(E$11)/SUM(E$6:E$13)*N44</f>
         <v>2582.1231033841427</v>
       </c>
       <c r="U44" s="113">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>2385.6110070402383</v>
       </c>
       <c r="V44" s="121">
@@ -10871,11 +10871,11 @@
         <v>7.4513659633715965E-2</v>
       </c>
       <c r="W44" s="121">
-        <f t="shared" ref="W44:X44" si="30">SUM(E$11)/SUM(E$6:E$13)*Q44</f>
+        <f t="shared" ref="W44:X44" si="31">SUM(E$11)/SUM(E$6:E$13)*Q44</f>
         <v>6.4070400320756282E-2</v>
       </c>
       <c r="X44" s="121">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>7.1161885518135765E-2</v>
       </c>
     </row>
@@ -10891,7 +10891,7 @@
         <v>4565</v>
       </c>
       <c r="G45" s="114">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>13926</v>
       </c>
       <c r="H45" s="114">
@@ -10905,15 +10905,15 @@
       </c>
       <c r="L45" s="114"/>
       <c r="M45" s="114">
-        <f t="shared" ref="M45:M57" si="31">AVERAGE(G45:I45)</f>
+        <f t="shared" ref="M45:M57" si="32">AVERAGE(G45:I45)</f>
         <v>19363</v>
       </c>
       <c r="N45" s="114">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>15409.3</v>
       </c>
       <c r="O45" s="114">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>12533.4</v>
       </c>
       <c r="P45" s="122">
@@ -10933,11 +10933,11 @@
         <v>2615.298056941107</v>
       </c>
       <c r="T45" s="113">
-        <f t="shared" ref="T45" si="32">SUM(E$11)/SUM(E$6:E$13)*N45</f>
+        <f t="shared" ref="T45" si="33">SUM(E$11)/SUM(E$6:E$13)*N45</f>
         <v>1781.4989226026787</v>
       </c>
       <c r="U45" s="113">
-        <f t="shared" ref="U45" si="33">SUM(F$11)/SUM(F$6:F$13)*O45</f>
+        <f t="shared" ref="U45" si="34">SUM(F$11)/SUM(F$6:F$13)*O45</f>
         <v>1636.2302444859317</v>
       </c>
       <c r="V45" s="121">
@@ -10945,11 +10945,11 @@
         <v>6.9831066763315575E-2</v>
       </c>
       <c r="W45" s="121">
-        <f t="shared" ref="W45" si="34">SUM(E$11)/SUM(E$6:E$13)*Q45</f>
+        <f t="shared" ref="W45" si="35">SUM(E$11)/SUM(E$6:E$13)*Q45</f>
         <v>5.9437113518890035E-2</v>
       </c>
       <c r="X45" s="121">
-        <f t="shared" ref="X45" si="35">SUM(F$11)/SUM(F$6:F$13)*R45</f>
+        <f t="shared" ref="X45" si="36">SUM(F$11)/SUM(F$6:F$13)*R45</f>
         <v>6.7752568250727771E-2</v>
       </c>
     </row>
@@ -10965,7 +10965,7 @@
         <v>3804</v>
       </c>
       <c r="G46" s="115">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>13165</v>
       </c>
       <c r="H46" s="115">
@@ -10980,15 +10980,15 @@
       </c>
       <c r="L46" s="115"/>
       <c r="M46" s="115">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>12682.5</v>
       </c>
       <c r="N46" s="115">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>10160.5</v>
       </c>
       <c r="O46" s="115">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>11848.5</v>
       </c>
       <c r="P46" s="120">
@@ -11020,11 +11020,11 @@
         <v>3.4994684514341713E-2</v>
       </c>
       <c r="W46" s="120">
-        <f t="shared" ref="W46:X46" si="36">E11/SUM(E6:E13)*Q46</f>
+        <f t="shared" ref="W46:X46" si="37">E11/SUM(E6:E13)*Q46</f>
         <v>2.9337023697179571E-2</v>
       </c>
       <c r="X46" s="120">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>3.6794477883422452E-2</v>
       </c>
     </row>
@@ -11040,7 +11040,7 @@
         <v>6086</v>
       </c>
       <c r="G47" s="114">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>34169</v>
       </c>
       <c r="H47" s="114"/>
@@ -11049,15 +11049,15 @@
       <c r="K47" s="114"/>
       <c r="L47" s="114"/>
       <c r="M47" s="114">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>34169</v>
       </c>
       <c r="N47" s="114">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>37585.9</v>
       </c>
       <c r="O47" s="114">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>30752.100000000002</v>
       </c>
       <c r="P47" s="122">
@@ -11077,11 +11077,11 @@
         <v>2280.8985892319106</v>
       </c>
       <c r="T47" s="113">
-        <f t="shared" ref="T47" si="37">SUM(E$12)/SUM(E$6:E$13)*N47</f>
+        <f t="shared" ref="T47" si="38">SUM(E$12)/SUM(E$6:E$13)*N47</f>
         <v>2308.4294549566052</v>
       </c>
       <c r="U47" s="113">
-        <f t="shared" ref="U47" si="38">SUM(F$12)/SUM(F$6:F$13)*O47</f>
+        <f t="shared" ref="U47" si="39">SUM(F$12)/SUM(F$6:F$13)*O47</f>
         <v>1921.2154160116083</v>
       </c>
       <c r="V47" s="121">
@@ -11089,11 +11089,11 @@
         <v>5.2348892601926177E-2</v>
       </c>
       <c r="W47" s="121">
-        <f t="shared" ref="W47" si="39">SUM(E$12)/SUM(E$6:E$13)*Q47</f>
+        <f t="shared" ref="W47" si="40">SUM(E$12)/SUM(E$6:E$13)*Q47</f>
         <v>4.8257406950146416E-2</v>
       </c>
       <c r="X47" s="121">
-        <f t="shared" ref="X47" si="40">SUM(F$12)/SUM(F$6:F$13)*R47</f>
+        <f t="shared" ref="X47" si="41">SUM(F$12)/SUM(F$6:F$13)*R47</f>
         <v>4.8388466845630869E-2</v>
       </c>
     </row>
@@ -11109,7 +11109,7 @@
         <v>5326</v>
       </c>
       <c r="G48" s="113">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>22176</v>
       </c>
       <c r="H48" s="113"/>
@@ -11118,15 +11118,15 @@
       <c r="K48" s="113"/>
       <c r="L48" s="113"/>
       <c r="M48" s="113">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>22176</v>
       </c>
       <c r="N48" s="113">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>24393.600000000002</v>
       </c>
       <c r="O48" s="113">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>19958.400000000001</v>
       </c>
       <c r="P48" s="121">
@@ -11146,11 +11146,11 @@
         <v>1480.3244787616509</v>
       </c>
       <c r="T48" s="113">
-        <f t="shared" ref="T48:U48" si="41">SUM(E$12)/SUM(E$6:E$13)*N48</f>
+        <f t="shared" ref="T48:U48" si="42">SUM(E$12)/SUM(E$6:E$13)*N48</f>
         <v>1498.1922676437027</v>
       </c>
       <c r="U48" s="113">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>1246.8867413583491</v>
       </c>
       <c r="V48" s="121">
@@ -11158,11 +11158,11 @@
         <v>4.3649312199432591E-2</v>
       </c>
       <c r="W48" s="121">
-        <f t="shared" ref="W48:X48" si="42">SUM(E$12)/SUM(E$6:E$13)*Q48</f>
+        <f t="shared" ref="W48:X48" si="43">SUM(E$12)/SUM(E$6:E$13)*Q48</f>
         <v>4.0030868653687851E-2</v>
       </c>
       <c r="X48" s="121">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>4.0577241203268805E-2</v>
       </c>
     </row>
@@ -11178,7 +11178,7 @@
         <v>4565</v>
       </c>
       <c r="G49" s="114">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>15798</v>
       </c>
       <c r="H49" s="114">
@@ -11192,15 +11192,15 @@
       <c r="K49" s="114"/>
       <c r="L49" s="114"/>
       <c r="M49" s="114">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>13399</v>
       </c>
       <c r="N49" s="114">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>26376.400000000001</v>
       </c>
       <c r="O49" s="114">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>14218.2</v>
       </c>
       <c r="P49" s="122">
@@ -11220,11 +11220,11 @@
         <v>894.42945936721503</v>
       </c>
       <c r="T49" s="113">
-        <f t="shared" ref="T49:T50" si="43">SUM(E$12)/SUM(E$6:E$13)*N49</f>
+        <f t="shared" ref="T49:T50" si="44">SUM(E$12)/SUM(E$6:E$13)*N49</f>
         <v>1619.9707516839401</v>
       </c>
       <c r="U49" s="113">
-        <f t="shared" ref="U49:U50" si="44">SUM(F$12)/SUM(F$6:F$13)*O49</f>
+        <f t="shared" ref="U49:U50" si="45">SUM(F$12)/SUM(F$6:F$13)*O49</f>
         <v>888.27185876529575</v>
       </c>
       <c r="V49" s="121">
@@ -11232,11 +11232,11 @@
         <v>4.1862661657399811E-2</v>
       </c>
       <c r="W49" s="121">
-        <f t="shared" ref="W49:W50" si="45">SUM(E$12)/SUM(E$6:E$13)*Q49</f>
+        <f t="shared" ref="W49:W50" si="46">SUM(E$12)/SUM(E$6:E$13)*Q49</f>
         <v>3.8108339757093442E-2</v>
       </c>
       <c r="X49" s="121">
-        <f t="shared" ref="X49:X50" si="46">SUM(F$12)/SUM(F$6:F$13)*R49</f>
+        <f t="shared" ref="X49:X50" si="47">SUM(F$12)/SUM(F$6:F$13)*R49</f>
         <v>3.9320180267811942E-2</v>
       </c>
     </row>
@@ -11252,7 +11252,7 @@
         <v>3804</v>
       </c>
       <c r="G50" s="114">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>11293</v>
       </c>
       <c r="H50" s="114">
@@ -11265,15 +11265,15 @@
       <c r="K50" s="114"/>
       <c r="L50" s="114"/>
       <c r="M50" s="114">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>10146.5</v>
       </c>
       <c r="N50" s="114">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>15711.150000000001</v>
       </c>
       <c r="O50" s="114">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>10163.700000000001</v>
       </c>
       <c r="P50" s="122">
@@ -11293,11 +11293,11 @@
         <v>677.31386741319852</v>
       </c>
       <c r="T50" s="113">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>964.93848574176673</v>
       </c>
       <c r="U50" s="113">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>634.96987599927104</v>
       </c>
       <c r="V50" s="121">
@@ -11305,11 +11305,11 @@
         <v>2.857078620501427E-2</v>
       </c>
       <c r="W50" s="121">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>2.5618654799750264E-2</v>
       </c>
       <c r="X50" s="121">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>2.7905517746048429E-2</v>
       </c>
     </row>
@@ -11325,7 +11325,7 @@
         <v>3043</v>
       </c>
       <c r="G51" s="115">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>8660</v>
       </c>
       <c r="H51" s="115">
@@ -11336,15 +11336,15 @@
       <c r="K51" s="115"/>
       <c r="L51" s="115"/>
       <c r="M51" s="115">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>4830</v>
       </c>
       <c r="N51" s="115">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>9526</v>
       </c>
       <c r="O51" s="115">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>7794</v>
       </c>
       <c r="P51" s="120">
@@ -11376,11 +11376,11 @@
         <v>1.5218510278777514E-2</v>
       </c>
       <c r="W51" s="120">
-        <f t="shared" ref="W51:X51" si="47">E12/SUM(E6:E13)*Q51</f>
+        <f t="shared" ref="W51:X51" si="48">E12/SUM(E6:E13)*Q51</f>
         <v>1.344559532603397E-2</v>
       </c>
       <c r="X51" s="120">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>1.4338900983817031E-2</v>
       </c>
     </row>
@@ -11396,7 +11396,7 @@
         <v>6086</v>
       </c>
       <c r="G52" s="114">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>36041</v>
       </c>
       <c r="H52" s="114"/>
@@ -11405,15 +11405,15 @@
       <c r="K52" s="114"/>
       <c r="L52" s="114"/>
       <c r="M52" s="114">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>36041</v>
       </c>
       <c r="N52" s="114">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>39645.100000000006</v>
       </c>
       <c r="O52" s="114">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>32436.9</v>
       </c>
       <c r="P52" s="122">
@@ -11447,7 +11447,7 @@
         <v>5326</v>
       </c>
       <c r="G53" s="113">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>22176</v>
       </c>
       <c r="H53" s="113"/>
@@ -11456,15 +11456,15 @@
       <c r="K53" s="113"/>
       <c r="L53" s="113"/>
       <c r="M53" s="113">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>22176</v>
       </c>
       <c r="N53" s="113">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>24393.600000000002</v>
       </c>
       <c r="O53" s="113">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>19958.400000000001</v>
       </c>
       <c r="P53" s="121">
@@ -11484,11 +11484,11 @@
         <v>1556.6052637176085</v>
       </c>
       <c r="T53" s="113">
-        <f t="shared" ref="T53:U53" si="48">SUM(E$13)/SUM(E$6:E$13)*N48</f>
+        <f t="shared" ref="T53:U53" si="49">SUM(E$13)/SUM(E$6:E$13)*N48</f>
         <v>2717.5942751454008</v>
       </c>
       <c r="U53" s="113">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>1538.1025473834977</v>
       </c>
       <c r="V53" s="121">
@@ -11496,11 +11496,11 @@
         <v>4.5557557929006579E-2</v>
       </c>
       <c r="W53" s="121">
-        <f t="shared" ref="W53:X53" si="49">SUM(E$13)/SUM(E$6:E$13)*Q53</f>
+        <f t="shared" ref="W53:X53" si="50">SUM(E$13)/SUM(E$6:E$13)*Q53</f>
         <v>7.2564406831507527E-2</v>
       </c>
       <c r="X53" s="121">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>5.1020288697720552E-2</v>
       </c>
     </row>
@@ -11516,7 +11516,7 @@
         <v>4565</v>
       </c>
       <c r="G54" s="114">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>15798</v>
       </c>
       <c r="H54" s="114"/>
@@ -11529,15 +11529,15 @@
         <v>8100</v>
       </c>
       <c r="M54" s="114">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>19649</v>
       </c>
       <c r="N54" s="114">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>17377.800000000003</v>
       </c>
       <c r="O54" s="114">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>11159.1</v>
       </c>
       <c r="P54" s="122">
@@ -11557,23 +11557,23 @@
         <v>940.51920673485915</v>
       </c>
       <c r="T54" s="113">
-        <f t="shared" ref="T54:T56" si="50">SUM(E$13)/SUM(E$6:E$13)*N49</f>
+        <f t="shared" ref="T54:T56" si="51">SUM(E$13)/SUM(E$6:E$13)*N49</f>
         <v>2938.4901629503288</v>
       </c>
       <c r="U54" s="113">
-        <f t="shared" ref="U54:U56" si="51">SUM(F$13)/SUM(F$6:F$13)*O49</f>
+        <f t="shared" ref="U54:U56" si="52">SUM(F$13)/SUM(F$6:F$13)*O49</f>
         <v>1095.7316036960901</v>
       </c>
       <c r="V54" s="121">
-        <f t="shared" ref="V54:V56" si="52">SUM(D$13)/SUM(D$6:D$13)*P54</f>
+        <f t="shared" ref="V54:V56" si="53">SUM(D$13)/SUM(D$6:D$13)*P54</f>
         <v>4.3652472553751862E-2</v>
       </c>
       <c r="W54" s="121">
-        <f t="shared" ref="W54:W56" si="53">SUM(E$13)/SUM(E$6:E$13)*Q54</f>
+        <f t="shared" ref="W54:W56" si="54">SUM(E$13)/SUM(E$6:E$13)*Q54</f>
         <v>6.907276803375445E-2</v>
       </c>
       <c r="X54" s="121">
-        <f t="shared" ref="X54:X56" si="54">SUM(F$13)/SUM(F$6:F$13)*R54</f>
+        <f t="shared" ref="X54:X56" si="55">SUM(F$13)/SUM(F$6:F$13)*R54</f>
         <v>4.9525094922424191E-2</v>
       </c>
     </row>
@@ -11589,7 +11589,7 @@
         <v>3804</v>
       </c>
       <c r="G55" s="114">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>11293</v>
       </c>
       <c r="H55" s="114">
@@ -11607,15 +11607,15 @@
         <v>4400</v>
       </c>
       <c r="M55" s="114">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>18864.333333333332</v>
       </c>
       <c r="N55" s="114">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>21853.15</v>
       </c>
       <c r="O55" s="114">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>7281.85</v>
       </c>
       <c r="P55" s="122">
@@ -11635,23 +11635,23 @@
         <v>712.21569752483379</v>
       </c>
       <c r="T55" s="113">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>1750.3169395230987</v>
       </c>
       <c r="U55" s="113">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>783.26984431826475</v>
       </c>
       <c r="V55" s="121">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>2.9479495276821064E-2</v>
       </c>
       <c r="W55" s="121">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>4.6389380207426861E-2</v>
       </c>
       <c r="X55" s="121">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>3.5948082171290856E-2</v>
       </c>
     </row>
@@ -11667,7 +11667,7 @@
         <v>3043</v>
       </c>
       <c r="G56" s="114">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>8660</v>
       </c>
       <c r="H56" s="114">
@@ -11682,15 +11682,15 @@
       </c>
       <c r="L56" s="114"/>
       <c r="M56" s="114">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>12830</v>
       </c>
       <c r="N56" s="114">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>17208.666666666668</v>
       </c>
       <c r="O56" s="114">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>7794</v>
       </c>
       <c r="P56" s="122">
@@ -11710,23 +11710,23 @@
         <v>339.03334342334279</v>
       </c>
       <c r="T56" s="113">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>1061.2538971301933</v>
       </c>
       <c r="U56" s="113">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>600.64791036891643</v>
       </c>
       <c r="V56" s="121">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>1.524211365405692E-2</v>
       </c>
       <c r="W56" s="121">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>2.4281038001972562E-2</v>
       </c>
       <c r="X56" s="121">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>1.9811457157685314E-2</v>
       </c>
     </row>
@@ -11750,15 +11750,15 @@
         <v>2200</v>
       </c>
       <c r="M57" s="116">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>2128</v>
       </c>
       <c r="N57" s="116">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1600</v>
       </c>
       <c r="O57" s="116">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1100</v>
       </c>
       <c r="P57" s="120">
@@ -11790,11 +11790,11 @@
         <v>-9.8521266588241329E-4</v>
       </c>
       <c r="W57" s="120">
-        <f t="shared" ref="W57:X57" si="55">E13/SUM(E6:E13)*Q57</f>
+        <f t="shared" ref="W57:X57" si="56">E13/SUM(E6:E13)*Q57</f>
         <v>-1.3844530588856169E-4</v>
       </c>
       <c r="X57" s="120">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>2.7562493385017966E-3</v>
       </c>
     </row>
@@ -11804,11 +11804,11 @@
         <v>9608.4735804205193</v>
       </c>
       <c r="T59" s="124">
-        <f t="shared" ref="T59:U59" si="56">SUM(T37,T39,T42,T46,T51,T57)</f>
+        <f t="shared" ref="T59:U59" si="57">SUM(T37,T39,T42,T46,T51,T57)</f>
         <v>14333.869646601945</v>
       </c>
       <c r="U59" s="124">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>11196.414691601361</v>
       </c>
       <c r="V59" s="123">
@@ -11816,11 +11816,11 @@
         <v>0.20172336037443986</v>
       </c>
       <c r="W59" s="123">
-        <f t="shared" ref="W59:X59" si="57">SUM(W37,W39,W42,W46,W51,W57)</f>
+        <f t="shared" ref="W59:X59" si="58">SUM(W37,W39,W42,W46,W51,W57)</f>
         <v>0.2000191767273756</v>
       </c>
       <c r="X59" s="123">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>0.21813305903885022</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update 30 year life retrofit inline with EU standards
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_RSD-Retrofit.xlsx
+++ b/SubRES_TMPL/SubRES_RSD-Retrofit.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B1F2D2-CD10-4963-81BA-5373FED5275A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302631FF-9E84-4A50-AF5A-7A15E1EDAA3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5640" yWindow="2250" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{61E3DBC4-3D48-40CE-BDD5-C17192DCDA09}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{61E3DBC4-3D48-40CE-BDD5-C17192DCDA09}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="59" r:id="rId1"/>
@@ -2483,6 +2483,9 @@
     <xf numFmtId="9" fontId="9" fillId="14" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="8" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2542,9 +2545,6 @@
     </xf>
     <xf numFmtId="0" fontId="38" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="8" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -4295,12 +4295,12 @@
       <c r="Z15" s="169"/>
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="207" t="s">
+      <c r="A16" s="208" t="s">
         <v>206</v>
       </c>
-      <c r="B16" s="207"/>
-      <c r="C16" s="207"/>
-      <c r="D16" s="207"/>
+      <c r="B16" s="208"/>
+      <c r="C16" s="208"/>
+      <c r="D16" s="208"/>
       <c r="E16" s="171"/>
       <c r="F16" s="171"/>
       <c r="G16" s="172"/>
@@ -4384,11 +4384,11 @@
       <c r="A19" s="176" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="206" t="s">
+      <c r="B19" s="207" t="s">
         <v>217</v>
       </c>
-      <c r="C19" s="206"/>
-      <c r="D19" s="206"/>
+      <c r="C19" s="207"/>
+      <c r="D19" s="207"/>
       <c r="E19" s="177"/>
       <c r="F19" s="177"/>
       <c r="G19" s="178"/>
@@ -4416,11 +4416,11 @@
       <c r="A20" s="176" t="s">
         <v>207</v>
       </c>
-      <c r="B20" s="206" t="s">
+      <c r="B20" s="207" t="s">
         <v>218</v>
       </c>
-      <c r="C20" s="206"/>
-      <c r="D20" s="206"/>
+      <c r="C20" s="207"/>
+      <c r="D20" s="207"/>
       <c r="E20" s="177"/>
       <c r="F20" s="177"/>
       <c r="G20" s="178"/>
@@ -4508,11 +4508,11 @@
       <c r="A23" s="176" t="s">
         <v>209</v>
       </c>
-      <c r="B23" s="206" t="s">
+      <c r="B23" s="207" t="s">
         <v>219</v>
       </c>
-      <c r="C23" s="206"/>
-      <c r="D23" s="206"/>
+      <c r="C23" s="207"/>
+      <c r="D23" s="207"/>
       <c r="E23" s="169"/>
       <c r="F23" s="169"/>
       <c r="G23" s="169"/>
@@ -4538,11 +4538,11 @@
     </row>
     <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="176"/>
-      <c r="B24" s="206" t="s">
+      <c r="B24" s="207" t="s">
         <v>220</v>
       </c>
-      <c r="C24" s="206"/>
-      <c r="D24" s="206"/>
+      <c r="C24" s="207"/>
+      <c r="D24" s="207"/>
       <c r="E24" s="169"/>
       <c r="F24" s="169"/>
       <c r="G24" s="169"/>
@@ -4598,11 +4598,11 @@
       <c r="A26" s="176" t="s">
         <v>210</v>
       </c>
-      <c r="B26" s="206" t="s">
+      <c r="B26" s="207" t="s">
         <v>219</v>
       </c>
-      <c r="C26" s="206"/>
-      <c r="D26" s="206"/>
+      <c r="C26" s="207"/>
+      <c r="D26" s="207"/>
       <c r="E26" s="169"/>
       <c r="F26" s="169"/>
       <c r="G26" s="169"/>
@@ -4628,11 +4628,11 @@
     </row>
     <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="176"/>
-      <c r="B27" s="206" t="s">
+      <c r="B27" s="207" t="s">
         <v>221</v>
       </c>
-      <c r="C27" s="206"/>
-      <c r="D27" s="206"/>
+      <c r="C27" s="207"/>
+      <c r="D27" s="207"/>
       <c r="E27" s="169"/>
       <c r="F27" s="169"/>
       <c r="G27" s="169"/>
@@ -4720,11 +4720,11 @@
       <c r="A30" s="176" t="s">
         <v>212</v>
       </c>
-      <c r="B30" s="208" t="s">
+      <c r="B30" s="209" t="s">
         <v>213</v>
       </c>
-      <c r="C30" s="206"/>
-      <c r="D30" s="206"/>
+      <c r="C30" s="207"/>
+      <c r="D30" s="207"/>
       <c r="E30" s="181"/>
       <c r="F30" s="181"/>
       <c r="G30" s="169"/>
@@ -4752,11 +4752,11 @@
       <c r="A31" s="176" t="s">
         <v>214</v>
       </c>
-      <c r="B31" s="206" t="s">
+      <c r="B31" s="207" t="s">
         <v>215</v>
       </c>
-      <c r="C31" s="206"/>
-      <c r="D31" s="206"/>
+      <c r="C31" s="207"/>
+      <c r="D31" s="207"/>
       <c r="E31" s="181"/>
       <c r="F31" s="181"/>
       <c r="G31" s="169"/>
@@ -6715,7 +6715,7 @@
   </sheetPr>
   <dimension ref="A1:U45"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -6734,17 +6734,17 @@
   <sheetData>
     <row r="1" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="209" t="s">
+      <c r="B2" s="210" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="210"/>
-      <c r="D2" s="210"/>
-      <c r="E2" s="211"/>
+      <c r="C2" s="211"/>
+      <c r="D2" s="211"/>
+      <c r="E2" s="212"/>
       <c r="F2" s="124"/>
-      <c r="H2" s="209" t="s">
+      <c r="H2" s="210" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="211"/>
+      <c r="I2" s="212"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="5"/>
@@ -7054,10 +7054,10 @@
         <v>72</v>
       </c>
       <c r="F15" s="126"/>
-      <c r="H15" s="209" t="s">
+      <c r="H15" s="210" t="s">
         <v>11</v>
       </c>
-      <c r="I15" s="211"/>
+      <c r="I15" s="212"/>
     </row>
     <row r="16" spans="2:21" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" s="17" t="s">
@@ -7131,12 +7131,12 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="212" t="s">
+      <c r="B20" s="213" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="213"/>
-      <c r="D20" s="213"/>
-      <c r="E20" s="214"/>
+      <c r="C20" s="214"/>
+      <c r="D20" s="214"/>
+      <c r="E20" s="215"/>
       <c r="F20" s="127"/>
     </row>
     <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -7347,17 +7347,17 @@
     </row>
     <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="38" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="209" t="s">
+      <c r="B38" s="210" t="s">
         <v>53</v>
       </c>
-      <c r="C38" s="210"/>
-      <c r="D38" s="210"/>
-      <c r="E38" s="211"/>
+      <c r="C38" s="211"/>
+      <c r="D38" s="211"/>
+      <c r="E38" s="212"/>
       <c r="F38" s="124"/>
-      <c r="H38" s="215" t="s">
+      <c r="H38" s="216" t="s">
         <v>50</v>
       </c>
-      <c r="I38" s="216"/>
+      <c r="I38" s="217"/>
     </row>
     <row r="39" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B39" s="49" t="s">
@@ -7464,7 +7464,7 @@
   <dimension ref="A1:Z58"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S31" sqref="S31"/>
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7660,7 +7660,7 @@
         <v>2020</v>
       </c>
       <c r="M7" s="202">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="N7" s="202">
         <f>U7</f>
@@ -7725,7 +7725,7 @@
         <v>2020</v>
       </c>
       <c r="M8" s="184">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="N8" s="184">
         <f t="shared" ref="N8:N9" si="3">U8</f>
@@ -7790,7 +7790,7 @@
         <v>2020</v>
       </c>
       <c r="M9" s="184">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="N9" s="184">
         <f t="shared" si="3"/>
@@ -7855,7 +7855,7 @@
         <v>2020</v>
       </c>
       <c r="M10" s="184">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="N10" s="184">
         <f t="shared" ref="N10:N12" si="7">U10</f>
@@ -7920,7 +7920,7 @@
         <v>2020</v>
       </c>
       <c r="M11" s="184">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="N11" s="184">
         <f t="shared" si="7"/>
@@ -7984,8 +7984,8 @@
       <c r="L12" s="195">
         <v>2020</v>
       </c>
-      <c r="M12" s="195">
-        <v>50</v>
+      <c r="M12" s="184">
+        <v>30</v>
       </c>
       <c r="N12" s="195">
         <f t="shared" si="7"/>
@@ -8049,8 +8049,8 @@
       <c r="L13" s="202">
         <v>2020</v>
       </c>
-      <c r="M13" s="202">
-        <v>50</v>
+      <c r="M13" s="184">
+        <v>30</v>
       </c>
       <c r="N13" s="202">
         <f>U13</f>
@@ -8114,7 +8114,7 @@
         <v>2020</v>
       </c>
       <c r="M14" s="184">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="N14" s="184">
         <f t="shared" ref="N14:N18" si="8">U14</f>
@@ -8179,7 +8179,7 @@
         <v>2020</v>
       </c>
       <c r="M15" s="184">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="N15" s="184">
         <f t="shared" si="8"/>
@@ -8244,7 +8244,7 @@
         <v>2020</v>
       </c>
       <c r="M16" s="184">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="N16" s="184">
         <f t="shared" si="8"/>
@@ -8309,7 +8309,7 @@
         <v>2020</v>
       </c>
       <c r="M17" s="184">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="N17" s="184">
         <f>U17</f>
@@ -8373,8 +8373,8 @@
       <c r="L18" s="195">
         <v>2020</v>
       </c>
-      <c r="M18" s="195">
-        <v>50</v>
+      <c r="M18" s="184">
+        <v>30</v>
       </c>
       <c r="N18" s="195">
         <f t="shared" si="8"/>
@@ -8438,8 +8438,8 @@
       <c r="L19" s="202">
         <v>2020</v>
       </c>
-      <c r="M19" s="202">
-        <v>50</v>
+      <c r="M19" s="184">
+        <v>30</v>
       </c>
       <c r="N19" s="202">
         <f>U19</f>
@@ -8504,7 +8504,7 @@
         <v>2020</v>
       </c>
       <c r="M20" s="184">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="N20" s="184">
         <f t="shared" ref="N20:N24" si="12">U20</f>
@@ -8569,7 +8569,7 @@
         <v>2020</v>
       </c>
       <c r="M21" s="184">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="N21" s="184">
         <f t="shared" si="12"/>
@@ -8634,7 +8634,7 @@
         <v>2020</v>
       </c>
       <c r="M22" s="184">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="N22" s="184">
         <f t="shared" si="12"/>
@@ -8699,7 +8699,7 @@
         <v>2020</v>
       </c>
       <c r="M23" s="184">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="N23" s="184">
         <f t="shared" si="12"/>
@@ -8763,8 +8763,8 @@
       <c r="L24" s="195">
         <v>2020</v>
       </c>
-      <c r="M24" s="195">
-        <v>50</v>
+      <c r="M24" s="184">
+        <v>30</v>
       </c>
       <c r="N24" s="195">
         <f t="shared" si="12"/>
@@ -9032,7 +9032,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AP60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
@@ -9063,33 +9063,33 @@
   <sheetData>
     <row r="1" spans="3:42" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="3:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L2" s="220" t="s">
+      <c r="L2" s="221" t="s">
         <v>167</v>
       </c>
-      <c r="M2" s="221"/>
-      <c r="N2" s="222"/>
-      <c r="O2" s="220" t="s">
+      <c r="M2" s="222"/>
+      <c r="N2" s="223"/>
+      <c r="O2" s="221" t="s">
         <v>168</v>
       </c>
-      <c r="P2" s="221"/>
-      <c r="Q2" s="222"/>
-      <c r="R2" s="220" t="s">
+      <c r="P2" s="222"/>
+      <c r="Q2" s="223"/>
+      <c r="R2" s="221" t="s">
         <v>178</v>
       </c>
-      <c r="S2" s="221"/>
-      <c r="T2" s="222"/>
+      <c r="S2" s="222"/>
+      <c r="T2" s="223"/>
       <c r="AD2" s="102" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="3" spans="3:42" ht="21.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="219" t="s">
+      <c r="C3" s="220" t="s">
         <v>156</v>
       </c>
-      <c r="D3" s="219"/>
-      <c r="E3" s="219"/>
-      <c r="F3" s="219"/>
-      <c r="G3" s="219"/>
+      <c r="D3" s="220"/>
+      <c r="E3" s="220"/>
+      <c r="F3" s="220"/>
+      <c r="G3" s="220"/>
       <c r="L3" s="72" t="s">
         <v>157</v>
       </c>
@@ -10652,15 +10652,15 @@
       <c r="C24" t="s">
         <v>186</v>
       </c>
-      <c r="F24" s="226">
+      <c r="F24" s="206">
         <f>F19/$D$14</f>
         <v>0.66874284103250692</v>
       </c>
-      <c r="G24" s="226">
+      <c r="G24" s="206">
         <f t="shared" ref="G24:G25" si="13">G19/$E$14</f>
         <v>0.66661969404564347</v>
       </c>
-      <c r="H24" s="226">
+      <c r="H24" s="206">
         <f t="shared" ref="H24:H25" si="14">H19/$F$14</f>
         <v>0.66292692209580051</v>
       </c>
@@ -10687,7 +10687,7 @@
         <v>187</v>
       </c>
       <c r="F25" s="122">
-        <f t="shared" ref="F24:F25" si="15">F20/$D$14</f>
+        <f t="shared" ref="F25" si="15">F20/$D$14</f>
         <v>0.21034483540254412</v>
       </c>
       <c r="G25" s="122">
@@ -10727,40 +10727,40 @@
       <c r="A29" s="101" t="s">
         <v>170</v>
       </c>
-      <c r="C29" s="223" t="s">
+      <c r="C29" s="224" t="s">
         <v>155</v>
       </c>
-      <c r="D29" s="224"/>
-      <c r="E29" s="224"/>
-      <c r="F29" s="224"/>
-      <c r="G29" s="225"/>
-      <c r="H29" s="223" t="s">
+      <c r="D29" s="225"/>
+      <c r="E29" s="225"/>
+      <c r="F29" s="225"/>
+      <c r="G29" s="226"/>
+      <c r="H29" s="224" t="s">
         <v>174</v>
       </c>
-      <c r="I29" s="224"/>
-      <c r="J29" s="224"/>
-      <c r="K29" s="224"/>
-      <c r="L29" s="225"/>
-      <c r="M29" s="217" t="s">
+      <c r="I29" s="225"/>
+      <c r="J29" s="225"/>
+      <c r="K29" s="225"/>
+      <c r="L29" s="226"/>
+      <c r="M29" s="218" t="s">
         <v>182</v>
       </c>
-      <c r="N29" s="218"/>
-      <c r="O29" s="218"/>
-      <c r="P29" s="217" t="s">
+      <c r="N29" s="219"/>
+      <c r="O29" s="219"/>
+      <c r="P29" s="218" t="s">
         <v>183</v>
       </c>
-      <c r="Q29" s="218"/>
-      <c r="R29" s="218"/>
-      <c r="S29" s="217" t="s">
+      <c r="Q29" s="219"/>
+      <c r="R29" s="219"/>
+      <c r="S29" s="218" t="s">
         <v>184</v>
       </c>
-      <c r="T29" s="218"/>
-      <c r="U29" s="218"/>
-      <c r="V29" s="217" t="s">
+      <c r="T29" s="219"/>
+      <c r="U29" s="219"/>
+      <c r="V29" s="218" t="s">
         <v>184</v>
       </c>
-      <c r="W29" s="218"/>
-      <c r="X29" s="218"/>
+      <c r="W29" s="219"/>
+      <c r="X29" s="219"/>
     </row>
     <row r="30" spans="1:42" ht="21" x14ac:dyDescent="0.2">
       <c r="A30" s="100" t="s">

</xml_diff>

<commit_message>
Update RTFT and Scen as Ambient is only coming through at HLI2
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_RSD-Retrofit.xlsx
+++ b/SubRES_TMPL/SubRES_RSD-Retrofit.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B37598E5-9EA2-43EB-AD89-A21761BE9F5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6083A2CF-886C-4B89-97DE-9D0B424E7539}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{61E3DBC4-3D48-40CE-BDD5-C17192DCDA09}"/>
   </bookViews>
@@ -2492,6 +2492,9 @@
     <xf numFmtId="167" fontId="0" fillId="8" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2551,9 +2554,6 @@
     </xf>
     <xf numFmtId="0" fontId="38" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -4304,12 +4304,12 @@
       <c r="Z15" s="169"/>
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="208" t="s">
+      <c r="A16" s="209" t="s">
         <v>206</v>
       </c>
-      <c r="B16" s="208"/>
-      <c r="C16" s="208"/>
-      <c r="D16" s="208"/>
+      <c r="B16" s="209"/>
+      <c r="C16" s="209"/>
+      <c r="D16" s="209"/>
       <c r="E16" s="171"/>
       <c r="F16" s="171"/>
       <c r="G16" s="172"/>
@@ -4393,11 +4393,11 @@
       <c r="A19" s="176" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="207" t="s">
+      <c r="B19" s="208" t="s">
         <v>217</v>
       </c>
-      <c r="C19" s="207"/>
-      <c r="D19" s="207"/>
+      <c r="C19" s="208"/>
+      <c r="D19" s="208"/>
       <c r="E19" s="177"/>
       <c r="F19" s="177"/>
       <c r="G19" s="178"/>
@@ -4425,11 +4425,11 @@
       <c r="A20" s="176" t="s">
         <v>207</v>
       </c>
-      <c r="B20" s="207" t="s">
+      <c r="B20" s="208" t="s">
         <v>218</v>
       </c>
-      <c r="C20" s="207"/>
-      <c r="D20" s="207"/>
+      <c r="C20" s="208"/>
+      <c r="D20" s="208"/>
       <c r="E20" s="177"/>
       <c r="F20" s="177"/>
       <c r="G20" s="178"/>
@@ -4517,11 +4517,11 @@
       <c r="A23" s="176" t="s">
         <v>209</v>
       </c>
-      <c r="B23" s="207" t="s">
+      <c r="B23" s="208" t="s">
         <v>219</v>
       </c>
-      <c r="C23" s="207"/>
-      <c r="D23" s="207"/>
+      <c r="C23" s="208"/>
+      <c r="D23" s="208"/>
       <c r="E23" s="169"/>
       <c r="F23" s="169"/>
       <c r="G23" s="169"/>
@@ -4547,11 +4547,11 @@
     </row>
     <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="176"/>
-      <c r="B24" s="207" t="s">
+      <c r="B24" s="208" t="s">
         <v>220</v>
       </c>
-      <c r="C24" s="207"/>
-      <c r="D24" s="207"/>
+      <c r="C24" s="208"/>
+      <c r="D24" s="208"/>
       <c r="E24" s="169"/>
       <c r="F24" s="169"/>
       <c r="G24" s="169"/>
@@ -4607,11 +4607,11 @@
       <c r="A26" s="176" t="s">
         <v>210</v>
       </c>
-      <c r="B26" s="207" t="s">
+      <c r="B26" s="208" t="s">
         <v>219</v>
       </c>
-      <c r="C26" s="207"/>
-      <c r="D26" s="207"/>
+      <c r="C26" s="208"/>
+      <c r="D26" s="208"/>
       <c r="E26" s="169"/>
       <c r="F26" s="169"/>
       <c r="G26" s="169"/>
@@ -4637,11 +4637,11 @@
     </row>
     <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="176"/>
-      <c r="B27" s="207" t="s">
+      <c r="B27" s="208" t="s">
         <v>221</v>
       </c>
-      <c r="C27" s="207"/>
-      <c r="D27" s="207"/>
+      <c r="C27" s="208"/>
+      <c r="D27" s="208"/>
       <c r="E27" s="169"/>
       <c r="F27" s="169"/>
       <c r="G27" s="169"/>
@@ -4729,11 +4729,11 @@
       <c r="A30" s="176" t="s">
         <v>212</v>
       </c>
-      <c r="B30" s="209" t="s">
+      <c r="B30" s="210" t="s">
         <v>213</v>
       </c>
-      <c r="C30" s="207"/>
-      <c r="D30" s="207"/>
+      <c r="C30" s="208"/>
+      <c r="D30" s="208"/>
       <c r="E30" s="181"/>
       <c r="F30" s="181"/>
       <c r="G30" s="169"/>
@@ -4761,11 +4761,11 @@
       <c r="A31" s="176" t="s">
         <v>214</v>
       </c>
-      <c r="B31" s="207" t="s">
+      <c r="B31" s="208" t="s">
         <v>215</v>
       </c>
-      <c r="C31" s="207"/>
-      <c r="D31" s="207"/>
+      <c r="C31" s="208"/>
+      <c r="D31" s="208"/>
       <c r="E31" s="181"/>
       <c r="F31" s="181"/>
       <c r="G31" s="169"/>
@@ -6743,17 +6743,17 @@
   <sheetData>
     <row r="1" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="210" t="s">
+      <c r="B2" s="211" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="211"/>
-      <c r="D2" s="211"/>
-      <c r="E2" s="212"/>
+      <c r="C2" s="212"/>
+      <c r="D2" s="212"/>
+      <c r="E2" s="213"/>
       <c r="F2" s="124"/>
-      <c r="H2" s="210" t="s">
+      <c r="H2" s="211" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="212"/>
+      <c r="I2" s="213"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="5"/>
@@ -7063,10 +7063,10 @@
         <v>72</v>
       </c>
       <c r="F15" s="126"/>
-      <c r="H15" s="210" t="s">
+      <c r="H15" s="211" t="s">
         <v>11</v>
       </c>
-      <c r="I15" s="212"/>
+      <c r="I15" s="213"/>
     </row>
     <row r="16" spans="2:21" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" s="17" t="s">
@@ -7140,12 +7140,12 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="213" t="s">
+      <c r="B20" s="214" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="214"/>
-      <c r="D20" s="214"/>
-      <c r="E20" s="215"/>
+      <c r="C20" s="215"/>
+      <c r="D20" s="215"/>
+      <c r="E20" s="216"/>
       <c r="F20" s="127"/>
     </row>
     <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -7356,17 +7356,17 @@
     </row>
     <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="38" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="210" t="s">
+      <c r="B38" s="211" t="s">
         <v>53</v>
       </c>
-      <c r="C38" s="211"/>
-      <c r="D38" s="211"/>
-      <c r="E38" s="212"/>
+      <c r="C38" s="212"/>
+      <c r="D38" s="212"/>
+      <c r="E38" s="213"/>
       <c r="F38" s="124"/>
-      <c r="H38" s="216" t="s">
+      <c r="H38" s="217" t="s">
         <v>50</v>
       </c>
-      <c r="I38" s="217"/>
+      <c r="I38" s="218"/>
     </row>
     <row r="39" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B39" s="49" t="s">
@@ -7472,8 +7472,8 @@
   </sheetPr>
   <dimension ref="A1:Z58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S30" sqref="S30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7704,7 +7704,7 @@
         <f>S7*T7</f>
         <v>7.7661668114821741E-4</v>
       </c>
-      <c r="V7" s="227"/>
+      <c r="V7" s="207"/>
     </row>
     <row r="8" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="68" t="s">
@@ -7770,7 +7770,7 @@
         <f>S8*T8</f>
         <v>5.6507961350996572E-4</v>
       </c>
-      <c r="V8" s="227"/>
+      <c r="V8" s="207"/>
     </row>
     <row r="9" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="63" t="s">
@@ -7836,7 +7836,7 @@
         <f t="shared" ref="U9:U12" si="6">S9*T9</f>
         <v>4.1735599619472851E-3</v>
       </c>
-      <c r="V9" s="227"/>
+      <c r="V9" s="207"/>
     </row>
     <row r="10" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="68" t="s">
@@ -7902,7 +7902,7 @@
         <f t="shared" si="6"/>
         <v>8.2884518803990805E-3</v>
       </c>
-      <c r="V10" s="227">
+      <c r="V10" s="207">
         <v>0.1</v>
       </c>
     </row>
@@ -7950,7 +7950,7 @@
       </c>
       <c r="O11" s="196">
         <f>(Data!O48/1000)*(1+V11)</f>
-        <v>24.948</v>
+        <v>23.95008</v>
       </c>
       <c r="P11" s="186"/>
       <c r="Q11" s="186" t="s">
@@ -7970,8 +7970,8 @@
         <f t="shared" si="6"/>
         <v>1.3423627595443485E-2</v>
       </c>
-      <c r="V11" s="227">
-        <v>0.25</v>
+      <c r="V11" s="207">
+        <v>0.2</v>
       </c>
     </row>
     <row r="12" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -8018,7 +8018,7 @@
       </c>
       <c r="O12" s="196">
         <f>(Data!O53/1000)*(1+V12)</f>
-        <v>31.933440000000004</v>
+        <v>26.943840000000002</v>
       </c>
       <c r="P12" s="186"/>
       <c r="Q12" s="197" t="s">
@@ -8038,8 +8038,8 @@
         <f t="shared" si="6"/>
         <v>1.6533815454634553E-2</v>
       </c>
-      <c r="V12" s="227">
-        <v>0.6</v>
+      <c r="V12" s="207">
+        <v>0.35</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -8105,7 +8105,7 @@
         <f>S13*T13</f>
         <v>1.7351329068959851E-3</v>
       </c>
-      <c r="V13" s="227"/>
+      <c r="V13" s="207"/>
     </row>
     <row r="14" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="68" t="s">
@@ -8171,7 +8171,7 @@
         <f>S14*T14</f>
         <v>1.4767673624826536E-3</v>
       </c>
-      <c r="V14" s="227"/>
+      <c r="V14" s="207"/>
     </row>
     <row r="15" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="63" t="s">
@@ -8237,7 +8237,7 @@
         <f t="shared" ref="U15:U18" si="11">S15*T15</f>
         <v>1.158897873793953E-2</v>
       </c>
-      <c r="V15" s="227"/>
+      <c r="V15" s="207"/>
     </row>
     <row r="16" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="68" t="s">
@@ -8303,7 +8303,7 @@
         <f t="shared" si="11"/>
         <v>2.2075128651129185E-2</v>
       </c>
-      <c r="V16" s="227">
+      <c r="V16" s="207">
         <v>0.1</v>
       </c>
     </row>
@@ -8351,7 +8351,7 @@
       </c>
       <c r="O17" s="196">
         <f>(Data!M48/1000)*(1+V17)</f>
-        <v>27.72</v>
+        <v>26.611199999999997</v>
       </c>
       <c r="P17" s="186"/>
       <c r="Q17" s="186" t="s">
@@ -8371,8 +8371,8 @@
         <f t="shared" si="11"/>
         <v>3.3422042455488611E-2</v>
       </c>
-      <c r="V17" s="227">
-        <v>0.25</v>
+      <c r="V17" s="207">
+        <v>0.2</v>
       </c>
     </row>
     <row r="18" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -8419,7 +8419,7 @@
       </c>
       <c r="O18" s="196">
         <f>(Data!M53/1000)*(1+V18)</f>
-        <v>35.4816</v>
+        <v>29.9376</v>
       </c>
       <c r="P18" s="186"/>
       <c r="Q18" s="197" t="s">
@@ -8439,8 +8439,8 @@
         <f t="shared" si="11"/>
         <v>3.4292348738938973E-2</v>
       </c>
-      <c r="V18" s="227">
-        <v>0.6</v>
+      <c r="V18" s="207">
+        <v>0.35</v>
       </c>
     </row>
     <row r="19" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -8507,7 +8507,7 @@
         <f>S19*T19</f>
         <v>4.7302606585568566E-3</v>
       </c>
-      <c r="V19" s="227"/>
+      <c r="V19" s="207"/>
     </row>
     <row r="20" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="68" t="s">
@@ -8573,7 +8573,7 @@
         <f>S20*T20</f>
         <v>3.4880235913390704E-3</v>
       </c>
-      <c r="V20" s="227"/>
+      <c r="V20" s="207"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="63" t="s">
@@ -8639,7 +8639,7 @@
         <f t="shared" ref="U21:U24" si="15">S21*T21</f>
         <v>1.9945744160653683E-2</v>
       </c>
-      <c r="V21" s="227"/>
+      <c r="V21" s="207"/>
     </row>
     <row r="22" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="68" t="s">
@@ -8705,7 +8705,7 @@
         <f t="shared" si="15"/>
         <v>3.4489478571996135E-2</v>
       </c>
-      <c r="V22" s="227">
+      <c r="V22" s="207">
         <v>0.1</v>
       </c>
     </row>
@@ -8753,7 +8753,7 @@
       </c>
       <c r="O23" s="196">
         <f>(Data!N48/1000)*(1+V23)</f>
-        <v>30.492000000000004</v>
+        <v>29.272320000000001</v>
       </c>
       <c r="P23" s="186"/>
       <c r="Q23" s="186" t="s">
@@ -8773,8 +8773,8 @@
         <f t="shared" si="15"/>
         <v>4.939185199641144E-2</v>
       </c>
-      <c r="V23" s="227">
-        <v>0.25</v>
+      <c r="V23" s="207">
+        <v>0.2</v>
       </c>
     </row>
     <row r="24" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -8821,7 +8821,7 @@
       </c>
       <c r="O24" s="196">
         <f>(Data!N53/1000)*(1+V24)</f>
-        <v>39.02976000000001</v>
+        <v>32.931360000000005</v>
       </c>
       <c r="P24" s="186"/>
       <c r="Q24" s="197" t="s">
@@ -8841,8 +8841,8 @@
         <f t="shared" si="15"/>
         <v>5.2917082120671262E-2</v>
       </c>
-      <c r="V24" s="227">
-        <v>0.6</v>
+      <c r="V24" s="207">
+        <v>0.35</v>
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.2">
@@ -9115,33 +9115,33 @@
   <sheetData>
     <row r="1" spans="3:42" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="3:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L2" s="221" t="s">
+      <c r="L2" s="222" t="s">
         <v>167</v>
       </c>
-      <c r="M2" s="222"/>
-      <c r="N2" s="223"/>
-      <c r="O2" s="221" t="s">
+      <c r="M2" s="223"/>
+      <c r="N2" s="224"/>
+      <c r="O2" s="222" t="s">
         <v>168</v>
       </c>
-      <c r="P2" s="222"/>
-      <c r="Q2" s="223"/>
-      <c r="R2" s="221" t="s">
+      <c r="P2" s="223"/>
+      <c r="Q2" s="224"/>
+      <c r="R2" s="222" t="s">
         <v>178</v>
       </c>
-      <c r="S2" s="222"/>
-      <c r="T2" s="223"/>
+      <c r="S2" s="223"/>
+      <c r="T2" s="224"/>
       <c r="AD2" s="102" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="3" spans="3:42" ht="21.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="220" t="s">
+      <c r="C3" s="221" t="s">
         <v>156</v>
       </c>
-      <c r="D3" s="220"/>
-      <c r="E3" s="220"/>
-      <c r="F3" s="220"/>
-      <c r="G3" s="220"/>
+      <c r="D3" s="221"/>
+      <c r="E3" s="221"/>
+      <c r="F3" s="221"/>
+      <c r="G3" s="221"/>
       <c r="L3" s="72" t="s">
         <v>157</v>
       </c>
@@ -10779,40 +10779,40 @@
       <c r="A29" s="101" t="s">
         <v>170</v>
       </c>
-      <c r="C29" s="224" t="s">
+      <c r="C29" s="225" t="s">
         <v>155</v>
       </c>
-      <c r="D29" s="225"/>
-      <c r="E29" s="225"/>
-      <c r="F29" s="225"/>
-      <c r="G29" s="226"/>
-      <c r="H29" s="224" t="s">
+      <c r="D29" s="226"/>
+      <c r="E29" s="226"/>
+      <c r="F29" s="226"/>
+      <c r="G29" s="227"/>
+      <c r="H29" s="225" t="s">
         <v>174</v>
       </c>
-      <c r="I29" s="225"/>
-      <c r="J29" s="225"/>
-      <c r="K29" s="225"/>
-      <c r="L29" s="226"/>
-      <c r="M29" s="218" t="s">
+      <c r="I29" s="226"/>
+      <c r="J29" s="226"/>
+      <c r="K29" s="226"/>
+      <c r="L29" s="227"/>
+      <c r="M29" s="219" t="s">
         <v>182</v>
       </c>
-      <c r="N29" s="219"/>
-      <c r="O29" s="219"/>
-      <c r="P29" s="218" t="s">
+      <c r="N29" s="220"/>
+      <c r="O29" s="220"/>
+      <c r="P29" s="219" t="s">
         <v>183</v>
       </c>
-      <c r="Q29" s="219"/>
-      <c r="R29" s="219"/>
-      <c r="S29" s="218" t="s">
+      <c r="Q29" s="220"/>
+      <c r="R29" s="220"/>
+      <c r="S29" s="219" t="s">
         <v>184</v>
       </c>
-      <c r="T29" s="219"/>
-      <c r="U29" s="219"/>
-      <c r="V29" s="218" t="s">
+      <c r="T29" s="220"/>
+      <c r="U29" s="220"/>
+      <c r="V29" s="219" t="s">
         <v>184</v>
       </c>
-      <c r="W29" s="219"/>
-      <c r="X29" s="219"/>
+      <c r="W29" s="220"/>
+      <c r="X29" s="220"/>
     </row>
     <row r="30" spans="1:42" ht="21" x14ac:dyDescent="0.2">
       <c r="A30" s="100" t="s">

</xml_diff>